<commit_message>
fixed our macine learning model
</commit_message>
<xml_diff>
--- a/frequencyVSdecreaseloss.xlsx
+++ b/frequencyVSdecreaseloss.xlsx
@@ -545,1223 +545,1223 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9501091172944235</v>
+        <v>0.9501092022737112</v>
       </c>
       <c r="C2" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D2" t="n">
-        <v>212160.7233467327</v>
+        <v>25589.4806700495</v>
       </c>
       <c r="E2" t="n">
-        <v>160.3432390030357</v>
+        <v>52.97119374088652</v>
       </c>
       <c r="F2" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G2" t="n">
-        <v>192073.4172888405</v>
+        <v>19237.30880625597</v>
       </c>
       <c r="H2" t="n">
-        <v>128.1464088405191</v>
+        <v>42.78171825597019</v>
       </c>
       <c r="I2" t="n">
-        <v>0.950183072802</v>
+        <v>0.9502589232513458</v>
       </c>
       <c r="J2" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K2" t="n">
-        <v>300013.9035017732</v>
+        <v>34321.53825534342</v>
       </c>
       <c r="L2" t="n">
-        <v>-484.8136599605787</v>
+        <v>-97.27285739697982</v>
       </c>
       <c r="M2" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N2" t="n">
-        <v>279754.1473332178</v>
+        <v>27907.67033677495</v>
       </c>
       <c r="O2" t="n">
-        <v>-539.3044407821726</v>
+        <v>-121.6748406250517</v>
       </c>
       <c r="P2" t="n">
-        <v>0.9501238963354697</v>
+        <v>0.9501870131737353</v>
       </c>
       <c r="Q2" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R2" t="n">
-        <v>351891.8768245445</v>
+        <v>40652.72066808033</v>
       </c>
       <c r="S2" t="n">
-        <v>-15.56248833733844</v>
+        <v>-52.64015733044653</v>
       </c>
       <c r="T2" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U2" t="n">
-        <v>326341.6347841184</v>
+        <v>32565.50992723136</v>
       </c>
       <c r="V2" t="n">
-        <v>-62.06374788162066</v>
+        <v>-74.85992596863798</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>0.9501090475028166</v>
+        <v>0.9499582441688347</v>
       </c>
       <c r="C3" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D3" t="n">
-        <v>212163.3830854285</v>
+        <v>25979.43706564939</v>
       </c>
       <c r="E3" t="n">
-        <v>163.0029776988958</v>
+        <v>442.927589340783</v>
       </c>
       <c r="F3" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G3" t="n">
-        <v>192076.0976584196</v>
+        <v>19641.34098657242</v>
       </c>
       <c r="H3" t="n">
-        <v>130.8267784195777</v>
+        <v>446.8138985724181</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9505520321816386</v>
+        <v>0.9504476609195637</v>
       </c>
       <c r="J3" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K3" t="n">
-        <v>288754.0510387286</v>
+        <v>33673.71281025065</v>
       </c>
       <c r="L3" t="n">
-        <v>-11744.66612300515</v>
+        <v>-745.0983024897505</v>
       </c>
       <c r="M3" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N3" t="n">
-        <v>268383.4482505456</v>
+        <v>27241.92276560219</v>
       </c>
       <c r="O3" t="n">
-        <v>-11910.00352345442</v>
+        <v>-787.4224117978119</v>
       </c>
       <c r="P3" t="n">
-        <v>0.9501267522249324</v>
+        <v>0.9501705255654982</v>
       </c>
       <c r="Q3" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R3" t="n">
-        <v>351761.9712278971</v>
+        <v>40748.56614813589</v>
       </c>
       <c r="S3" t="n">
-        <v>-145.4680849846918</v>
+        <v>43.20532272511628</v>
       </c>
       <c r="T3" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U3" t="n">
-        <v>326210.6550199011</v>
+        <v>32663.31998567862</v>
       </c>
       <c r="V3" t="n">
-        <v>-193.0435120989569</v>
+        <v>22.95013247862153</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>0.9501061322934581</v>
+        <v>0.947826191771591</v>
       </c>
       <c r="C4" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D4" t="n">
-        <v>212193.2526748529</v>
+        <v>28376.60823449296</v>
       </c>
       <c r="E4" t="n">
-        <v>192.8725671232969</v>
+        <v>2840.098758184355</v>
       </c>
       <c r="F4" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G4" t="n">
-        <v>192106.8289607194</v>
+        <v>22230.00163284579</v>
       </c>
       <c r="H4" t="n">
-        <v>161.5580807193764</v>
+        <v>3035.474544845791</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9509630321116597</v>
+        <v>0.9504923485859001</v>
       </c>
       <c r="J4" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K4" t="n">
-        <v>274533.0184772984</v>
+        <v>33531.87176602198</v>
       </c>
       <c r="L4" t="n">
-        <v>-25965.69868443534</v>
+        <v>-886.9393467184127</v>
       </c>
       <c r="M4" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N4" t="n">
-        <v>254037.2914408746</v>
+        <v>27095.82148664376</v>
       </c>
       <c r="O4" t="n">
-        <v>-26256.16033312544</v>
+        <v>-933.5236907562467</v>
       </c>
       <c r="P4" t="n">
-        <v>0.9501386616323357</v>
+        <v>0.9492428112301525</v>
       </c>
       <c r="Q4" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R4" t="n">
-        <v>350697.1228919991</v>
+        <v>43000.6989492728</v>
       </c>
       <c r="S4" t="n">
-        <v>-1210.316420882707</v>
+        <v>2295.33812386202</v>
       </c>
       <c r="T4" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U4" t="n">
-        <v>325141.3261618214</v>
+        <v>35024.26798922967</v>
       </c>
       <c r="V4" t="n">
-        <v>-1262.372370178637</v>
+        <v>2383.898136029671</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9503469076175962</v>
+        <v>0.951425903287602</v>
       </c>
       <c r="C5" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D5" t="n">
-        <v>209598.1622332539</v>
+        <v>23796.98493635857</v>
       </c>
       <c r="E5" t="n">
-        <v>-2402.217874475755</v>
+        <v>-1739.524539950035</v>
       </c>
       <c r="F5" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G5" t="n">
-        <v>189440.2814007709</v>
+        <v>17318.93446888218</v>
       </c>
       <c r="H5" t="n">
-        <v>-2504.989479229145</v>
+        <v>-1875.592619117822</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9510352585484164</v>
+        <v>0.9506213202672443</v>
       </c>
       <c r="J5" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K5" t="n">
-        <v>272594.6288852683</v>
+        <v>33208.08227929939</v>
       </c>
       <c r="L5" t="n">
-        <v>-27904.08827646548</v>
+        <v>-1210.728833441011</v>
       </c>
       <c r="M5" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N5" t="n">
-        <v>252076.7310095477</v>
+        <v>26759.7003693673</v>
       </c>
       <c r="O5" t="n">
-        <v>-28216.7207644523</v>
+        <v>-1269.644808032703</v>
       </c>
       <c r="P5" t="n">
-        <v>0.950294680426059</v>
+        <v>0.9509350723155203</v>
       </c>
       <c r="Q5" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R5" t="n">
-        <v>347765.9360567041</v>
+        <v>39713.57389501934</v>
       </c>
       <c r="S5" t="n">
-        <v>-4141.503256177646</v>
+        <v>-991.786930391434</v>
       </c>
       <c r="T5" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U5" t="n">
-        <v>322151.2761153771</v>
+        <v>31536.06419762421</v>
       </c>
       <c r="V5" t="n">
-        <v>-4252.422416622925</v>
+        <v>-1104.30565557579</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>0.95077125613669</v>
+        <v>0.9520822388284927</v>
       </c>
       <c r="C6" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D6" t="n">
-        <v>202757.8739627836</v>
+        <v>22568.60793068708</v>
       </c>
       <c r="E6" t="n">
-        <v>-9242.506144946034</v>
+        <v>-2967.901545621527</v>
       </c>
       <c r="F6" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G6" t="n">
-        <v>182472.6286710707</v>
+        <v>16025.64222367884</v>
       </c>
       <c r="H6" t="n">
-        <v>-9472.642208929319</v>
+        <v>-3168.884864321159</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9521326867605822</v>
+        <v>0.9519869931582354</v>
       </c>
       <c r="J6" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K6" t="n">
-        <v>241884.2935941395</v>
+        <v>29688.45536271131</v>
       </c>
       <c r="L6" t="n">
-        <v>-58614.42356759426</v>
+        <v>-4730.355750029092</v>
       </c>
       <c r="M6" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N6" t="n">
-        <v>221022.6101029175</v>
+        <v>23106.08568647636</v>
       </c>
       <c r="O6" t="n">
-        <v>-59270.84167108254</v>
+        <v>-4923.259490923643</v>
       </c>
       <c r="P6" t="n">
-        <v>0.950453967209071</v>
+        <v>0.950985027822744</v>
       </c>
       <c r="Q6" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R6" t="n">
-        <v>343943.9712509362</v>
+        <v>39637.12704559448</v>
       </c>
       <c r="S6" t="n">
-        <v>-7963.468061945634</v>
+        <v>-1068.233779816299</v>
       </c>
       <c r="T6" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U6" t="n">
-        <v>318268.8943947758</v>
+        <v>31453.50474909299</v>
       </c>
       <c r="V6" t="n">
-        <v>-8134.804137224215</v>
+        <v>-1186.865104107012</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9508485395588151</v>
+        <v>0.9524461563521174</v>
       </c>
       <c r="C7" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D7" t="n">
-        <v>200192.0421508207</v>
+        <v>21949.41225428852</v>
       </c>
       <c r="E7" t="n">
-        <v>-11808.33795690897</v>
+        <v>-3587.097222020086</v>
       </c>
       <c r="F7" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G7" t="n">
-        <v>179883.4021583563</v>
+        <v>15369.80226035527</v>
       </c>
       <c r="H7" t="n">
-        <v>-12061.8687216437</v>
+        <v>-3824.724827644732</v>
       </c>
       <c r="I7" t="n">
-        <v>0.952633604840836</v>
+        <v>0.9523408893579143</v>
       </c>
       <c r="J7" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K7" t="n">
-        <v>227640.3329764159</v>
+        <v>28796.48094694545</v>
       </c>
       <c r="L7" t="n">
-        <v>-72858.3841853179</v>
+        <v>-5622.330165794949</v>
       </c>
       <c r="M7" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N7" t="n">
-        <v>206617.2710721484</v>
+        <v>22178.33631873615</v>
       </c>
       <c r="O7" t="n">
-        <v>-73676.18070185158</v>
+        <v>-5851.008858663856</v>
       </c>
       <c r="P7" t="n">
-        <v>0.9518212694108429</v>
+        <v>0.95192279091625</v>
       </c>
       <c r="Q7" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R7" t="n">
-        <v>312878.4971253724</v>
+        <v>36784.10781181564</v>
       </c>
       <c r="S7" t="n">
-        <v>-39028.94218750938</v>
+        <v>-3921.253013595131</v>
       </c>
       <c r="T7" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U7" t="n">
-        <v>286671.0354547093</v>
+        <v>28483.75935475129</v>
       </c>
       <c r="V7" t="n">
-        <v>-39732.66307729069</v>
+        <v>-4156.610498448714</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>0.9508991564083724</v>
+        <v>0.9541310856143499</v>
       </c>
       <c r="C8" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D8" t="n">
-        <v>198133.7441383039</v>
+        <v>17718.41887428429</v>
       </c>
       <c r="E8" t="n">
-        <v>-13866.63596942576</v>
+        <v>-7818.09060202432</v>
       </c>
       <c r="F8" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G8" t="n">
-        <v>177809.7482181655</v>
+        <v>10962.7555177206</v>
       </c>
       <c r="H8" t="n">
-        <v>-14135.52266183455</v>
+        <v>-8231.771570279398</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9530021571771009</v>
+        <v>0.9530553295320467</v>
       </c>
       <c r="J8" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K8" t="n">
-        <v>214549.0848793174</v>
+        <v>26663.87068099071</v>
       </c>
       <c r="L8" t="n">
-        <v>-85949.63228241634</v>
+        <v>-7754.940431749688</v>
       </c>
       <c r="M8" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N8" t="n">
-        <v>193405.4326376391</v>
+        <v>19972.11720552375</v>
       </c>
       <c r="O8" t="n">
-        <v>-86888.01913636088</v>
+        <v>-8057.227971876251</v>
       </c>
       <c r="P8" t="n">
-        <v>0.952256830847301</v>
+        <v>0.9526934619300121</v>
       </c>
       <c r="Q8" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R8" t="n">
-        <v>295528.0676723787</v>
+        <v>33913.12725371122</v>
       </c>
       <c r="S8" t="n">
-        <v>-56379.37164050306</v>
+        <v>-6792.233571699551</v>
       </c>
       <c r="T8" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U8" t="n">
-        <v>269145.628594078</v>
+        <v>25513.93608652818</v>
       </c>
       <c r="V8" t="n">
-        <v>-57258.069937922</v>
+        <v>-7126.433766671824</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B9" t="n">
-        <v>0.9508991564083724</v>
+        <v>0.9541310856143499</v>
       </c>
       <c r="C9" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D9" t="n">
-        <v>198133.7441383039</v>
+        <v>17718.41887428429</v>
       </c>
       <c r="E9" t="n">
-        <v>-13866.63596942576</v>
+        <v>-7818.09060202432</v>
       </c>
       <c r="F9" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G9" t="n">
-        <v>177809.7482181655</v>
+        <v>10962.7555177206</v>
       </c>
       <c r="H9" t="n">
-        <v>-14135.52266183455</v>
+        <v>-8231.771570279398</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9530021571771009</v>
+        <v>0.9530553295320467</v>
       </c>
       <c r="J9" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K9" t="n">
-        <v>214549.0848793174</v>
+        <v>26663.87068099071</v>
       </c>
       <c r="L9" t="n">
-        <v>-85949.63228241634</v>
+        <v>-7754.940431749688</v>
       </c>
       <c r="M9" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N9" t="n">
-        <v>193405.4326376391</v>
+        <v>19972.11720552375</v>
       </c>
       <c r="O9" t="n">
-        <v>-86888.01913636088</v>
+        <v>-8057.227971876251</v>
       </c>
       <c r="P9" t="n">
-        <v>0.9524028023870822</v>
+        <v>0.9527579845560894</v>
       </c>
       <c r="Q9" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R9" t="n">
-        <v>288609.8350304586</v>
+        <v>33324.38896882621</v>
       </c>
       <c r="S9" t="n">
-        <v>-63297.60428242316</v>
+        <v>-7380.971856584569</v>
       </c>
       <c r="T9" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U9" t="n">
-        <v>262168.1504101177</v>
+        <v>24916.79885370818</v>
       </c>
       <c r="V9" t="n">
-        <v>-64235.54812188231</v>
+        <v>-7723.570999491825</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>0.9508991564083724</v>
+        <v>0.9541310856143499</v>
       </c>
       <c r="C10" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D10" t="n">
-        <v>198133.7441383039</v>
+        <v>17718.41887428429</v>
       </c>
       <c r="E10" t="n">
-        <v>-13866.63596942576</v>
+        <v>-7818.09060202432</v>
       </c>
       <c r="F10" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G10" t="n">
-        <v>177809.7482181655</v>
+        <v>10962.7555177206</v>
       </c>
       <c r="H10" t="n">
-        <v>-14135.52266183455</v>
+        <v>-8231.771570279398</v>
       </c>
       <c r="I10" t="n">
-        <v>0.9532206109016619</v>
+        <v>0.9535902205374004</v>
       </c>
       <c r="J10" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K10" t="n">
-        <v>206078.8698206702</v>
+        <v>24525.88066177466</v>
       </c>
       <c r="L10" t="n">
-        <v>-94419.84734106361</v>
+        <v>-9892.930450965734</v>
       </c>
       <c r="M10" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N10" t="n">
-        <v>184862.9804805614</v>
+        <v>17777.76299663002</v>
       </c>
       <c r="O10" t="n">
-        <v>-95430.47129343863</v>
+        <v>-10251.58218076998</v>
       </c>
       <c r="P10" t="n">
-        <v>0.9521412735119815</v>
+        <v>0.9526975140239827</v>
       </c>
       <c r="Q10" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R10" t="n">
-        <v>300315.435237021</v>
+        <v>33714.21018835801</v>
       </c>
       <c r="S10" t="n">
-        <v>-51592.00407586084</v>
+        <v>-6991.150637052764</v>
       </c>
       <c r="T10" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U10" t="n">
-        <v>273979.6808410597</v>
+        <v>25314.49212840313</v>
       </c>
       <c r="V10" t="n">
-        <v>-52424.01769094035</v>
+        <v>-7325.877724796876</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B11" t="n">
-        <v>0.9510343339289785</v>
+        <v>0.9545093407777331</v>
       </c>
       <c r="C11" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D11" t="n">
-        <v>193820.0528968952</v>
+        <v>16501.23922446569</v>
       </c>
       <c r="E11" t="n">
-        <v>-18180.32721083442</v>
+        <v>-9035.270251842914</v>
       </c>
       <c r="F11" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G11" t="n">
-        <v>173454.9165805015</v>
+        <v>9704.534628774378</v>
       </c>
       <c r="H11" t="n">
-        <v>-18490.35429949855</v>
+        <v>-9489.992459225625</v>
       </c>
       <c r="I11" t="n">
-        <v>0.95396831505491</v>
+        <v>0.9543746754332608</v>
       </c>
       <c r="J11" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K11" t="n">
-        <v>162103.707301646</v>
+        <v>20573.08287393989</v>
       </c>
       <c r="L11" t="n">
-        <v>-138395.0098600878</v>
+        <v>-13845.72823880051</v>
       </c>
       <c r="M11" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N11" t="n">
-        <v>140636.1767574072</v>
+        <v>13740.27783596959</v>
       </c>
       <c r="O11" t="n">
-        <v>-139657.2750165928</v>
+        <v>-14289.06734143041</v>
       </c>
       <c r="P11" t="n">
-        <v>0.9527735881763383</v>
+        <v>0.9530981600049149</v>
       </c>
       <c r="Q11" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R11" t="n">
-        <v>275220.3475144443</v>
+        <v>32078.95737517925</v>
       </c>
       <c r="S11" t="n">
-        <v>-76687.09179843753</v>
+        <v>-8626.403450231526</v>
       </c>
       <c r="T11" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U11" t="n">
-        <v>248626.7808909985</v>
+        <v>23626.76318557685</v>
       </c>
       <c r="V11" t="n">
-        <v>-77776.91764100146</v>
+        <v>-9013.606667623149</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B12" t="n">
-        <v>0.9510343339289785</v>
+        <v>0.9545093407777331</v>
       </c>
       <c r="C12" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D12" t="n">
-        <v>193820.0528968952</v>
+        <v>16501.23922446569</v>
       </c>
       <c r="E12" t="n">
-        <v>-18180.32721083442</v>
+        <v>-9035.270251842914</v>
       </c>
       <c r="F12" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G12" t="n">
-        <v>173454.9165805015</v>
+        <v>9704.534628774378</v>
       </c>
       <c r="H12" t="n">
-        <v>-18490.35429949855</v>
+        <v>-9489.992459225625</v>
       </c>
       <c r="I12" t="n">
-        <v>0.95396831505491</v>
+        <v>0.9543746754332608</v>
       </c>
       <c r="J12" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K12" t="n">
-        <v>162103.707301646</v>
+        <v>20573.08287393989</v>
       </c>
       <c r="L12" t="n">
-        <v>-138395.0098600878</v>
+        <v>-13845.72823880051</v>
       </c>
       <c r="M12" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N12" t="n">
-        <v>140636.1767574072</v>
+        <v>13740.27783596959</v>
       </c>
       <c r="O12" t="n">
-        <v>-139657.2750165928</v>
+        <v>-14289.06734143041</v>
       </c>
       <c r="P12" t="n">
-        <v>0.9527735881763383</v>
+        <v>0.9530981600049149</v>
       </c>
       <c r="Q12" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R12" t="n">
-        <v>275220.3475144443</v>
+        <v>32078.95737517925</v>
       </c>
       <c r="S12" t="n">
-        <v>-76687.09179843753</v>
+        <v>-8626.403450231526</v>
       </c>
       <c r="T12" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U12" t="n">
-        <v>248626.7808909985</v>
+        <v>23626.76318557685</v>
       </c>
       <c r="V12" t="n">
-        <v>-77776.91764100146</v>
+        <v>-9013.606667623149</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B13" t="n">
-        <v>0.9510343339289785</v>
+        <v>0.9545093407777331</v>
       </c>
       <c r="C13" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D13" t="n">
-        <v>193820.0528968952</v>
+        <v>16501.23922446569</v>
       </c>
       <c r="E13" t="n">
-        <v>-18180.32721083442</v>
+        <v>-9035.270251842914</v>
       </c>
       <c r="F13" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G13" t="n">
-        <v>173454.9165805015</v>
+        <v>9704.534628774378</v>
       </c>
       <c r="H13" t="n">
-        <v>-18490.35429949855</v>
+        <v>-9489.992459225625</v>
       </c>
       <c r="I13" t="n">
-        <v>0.95396831505491</v>
+        <v>0.9543746754332608</v>
       </c>
       <c r="J13" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K13" t="n">
-        <v>162103.707301646</v>
+        <v>20573.08287393989</v>
       </c>
       <c r="L13" t="n">
-        <v>-138395.0098600878</v>
+        <v>-13845.72823880051</v>
       </c>
       <c r="M13" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N13" t="n">
-        <v>140636.1767574072</v>
+        <v>13740.27783596959</v>
       </c>
       <c r="O13" t="n">
-        <v>-139657.2750165928</v>
+        <v>-14289.06734143041</v>
       </c>
       <c r="P13" t="n">
-        <v>0.9527735881763383</v>
+        <v>0.9530981600049149</v>
       </c>
       <c r="Q13" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R13" t="n">
-        <v>275220.3475144443</v>
+        <v>32078.95737517925</v>
       </c>
       <c r="S13" t="n">
-        <v>-76687.09179843753</v>
+        <v>-8626.403450231526</v>
       </c>
       <c r="T13" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U13" t="n">
-        <v>248626.7808909985</v>
+        <v>23626.76318557685</v>
       </c>
       <c r="V13" t="n">
-        <v>-77776.91764100146</v>
+        <v>-9013.606667623149</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B14" t="n">
-        <v>0.9510343339289785</v>
+        <v>0.9545093407777331</v>
       </c>
       <c r="C14" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D14" t="n">
-        <v>193820.0528968952</v>
+        <v>16501.23922446569</v>
       </c>
       <c r="E14" t="n">
-        <v>-18180.32721083442</v>
+        <v>-9035.270251842914</v>
       </c>
       <c r="F14" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G14" t="n">
-        <v>173454.9165805015</v>
+        <v>9704.534628774378</v>
       </c>
       <c r="H14" t="n">
-        <v>-18490.35429949855</v>
+        <v>-9489.992459225625</v>
       </c>
       <c r="I14" t="n">
-        <v>0.95396831505491</v>
+        <v>0.9543746754332608</v>
       </c>
       <c r="J14" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K14" t="n">
-        <v>162103.707301646</v>
+        <v>20573.08287393989</v>
       </c>
       <c r="L14" t="n">
-        <v>-138395.0098600878</v>
+        <v>-13845.72823880051</v>
       </c>
       <c r="M14" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N14" t="n">
-        <v>140636.1767574072</v>
+        <v>13740.27783596959</v>
       </c>
       <c r="O14" t="n">
-        <v>-139657.2750165928</v>
+        <v>-14289.06734143041</v>
       </c>
       <c r="P14" t="n">
-        <v>0.9527735881763383</v>
+        <v>0.9530981600049149</v>
       </c>
       <c r="Q14" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R14" t="n">
-        <v>275220.3475144443</v>
+        <v>32078.95737517925</v>
       </c>
       <c r="S14" t="n">
-        <v>-76687.09179843753</v>
+        <v>-8626.403450231526</v>
       </c>
       <c r="T14" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U14" t="n">
-        <v>248626.7808909985</v>
+        <v>23626.76318557685</v>
       </c>
       <c r="V14" t="n">
-        <v>-77776.91764100146</v>
+        <v>-9013.606667623149</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B15" t="n">
-        <v>0.9510343339289785</v>
+        <v>0.9545093407777331</v>
       </c>
       <c r="C15" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D15" t="n">
-        <v>193820.0528968952</v>
+        <v>16501.23922446569</v>
       </c>
       <c r="E15" t="n">
-        <v>-18180.32721083442</v>
+        <v>-9035.270251842914</v>
       </c>
       <c r="F15" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G15" t="n">
-        <v>173454.9165805015</v>
+        <v>9704.534628774378</v>
       </c>
       <c r="H15" t="n">
-        <v>-18490.35429949855</v>
+        <v>-9489.992459225625</v>
       </c>
       <c r="I15" t="n">
-        <v>0.95396831505491</v>
+        <v>0.9543746754332608</v>
       </c>
       <c r="J15" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K15" t="n">
-        <v>162103.707301646</v>
+        <v>20573.08287393989</v>
       </c>
       <c r="L15" t="n">
-        <v>-138395.0098600878</v>
+        <v>-13845.72823880051</v>
       </c>
       <c r="M15" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N15" t="n">
-        <v>140636.1767574072</v>
+        <v>13740.27783596959</v>
       </c>
       <c r="O15" t="n">
-        <v>-139657.2750165928</v>
+        <v>-14289.06734143041</v>
       </c>
       <c r="P15" t="n">
-        <v>0.9527735881763383</v>
+        <v>0.9530981600049149</v>
       </c>
       <c r="Q15" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R15" t="n">
-        <v>275220.3475144443</v>
+        <v>32078.95737517925</v>
       </c>
       <c r="S15" t="n">
-        <v>-76687.09179843753</v>
+        <v>-8626.403450231526</v>
       </c>
       <c r="T15" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U15" t="n">
-        <v>248626.7808909985</v>
+        <v>23626.76318557685</v>
       </c>
       <c r="V15" t="n">
-        <v>-77776.91764100146</v>
+        <v>-9013.606667623149</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B16" t="n">
-        <v>0.9510343339289785</v>
+        <v>0.9545093407777331</v>
       </c>
       <c r="C16" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D16" t="n">
-        <v>193820.0528968952</v>
+        <v>16501.23922446569</v>
       </c>
       <c r="E16" t="n">
-        <v>-18180.32721083442</v>
+        <v>-9035.270251842914</v>
       </c>
       <c r="F16" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G16" t="n">
-        <v>173454.9165805015</v>
+        <v>9704.534628774378</v>
       </c>
       <c r="H16" t="n">
-        <v>-18490.35429949855</v>
+        <v>-9489.992459225625</v>
       </c>
       <c r="I16" t="n">
-        <v>0.95396831505491</v>
+        <v>0.9543746754332608</v>
       </c>
       <c r="J16" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K16" t="n">
-        <v>162103.707301646</v>
+        <v>20573.08287393989</v>
       </c>
       <c r="L16" t="n">
-        <v>-138395.0098600878</v>
+        <v>-13845.72823880051</v>
       </c>
       <c r="M16" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N16" t="n">
-        <v>140636.1767574072</v>
+        <v>13740.27783596959</v>
       </c>
       <c r="O16" t="n">
-        <v>-139657.2750165928</v>
+        <v>-14289.06734143041</v>
       </c>
       <c r="P16" t="n">
-        <v>0.9527735881763383</v>
+        <v>0.9530981600049149</v>
       </c>
       <c r="Q16" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R16" t="n">
-        <v>275220.3475144443</v>
+        <v>32078.95737517925</v>
       </c>
       <c r="S16" t="n">
-        <v>-76687.09179843753</v>
+        <v>-8626.403450231526</v>
       </c>
       <c r="T16" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U16" t="n">
-        <v>248626.7808909985</v>
+        <v>23626.76318557685</v>
       </c>
       <c r="V16" t="n">
-        <v>-77776.91764100146</v>
+        <v>-9013.606667623149</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B17" t="n">
-        <v>0.9510343339289785</v>
+        <v>0.9545093407777331</v>
       </c>
       <c r="C17" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D17" t="n">
-        <v>193820.0528968952</v>
+        <v>16501.23922446569</v>
       </c>
       <c r="E17" t="n">
-        <v>-18180.32721083442</v>
+        <v>-9035.270251842914</v>
       </c>
       <c r="F17" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G17" t="n">
-        <v>173454.9165805015</v>
+        <v>9704.534628774378</v>
       </c>
       <c r="H17" t="n">
-        <v>-18490.35429949855</v>
+        <v>-9489.992459225625</v>
       </c>
       <c r="I17" t="n">
-        <v>0.95396831505491</v>
+        <v>0.9543746754332608</v>
       </c>
       <c r="J17" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K17" t="n">
-        <v>162103.707301646</v>
+        <v>20573.08287393989</v>
       </c>
       <c r="L17" t="n">
-        <v>-138395.0098600878</v>
+        <v>-13845.72823880051</v>
       </c>
       <c r="M17" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N17" t="n">
-        <v>140636.1767574072</v>
+        <v>13740.27783596959</v>
       </c>
       <c r="O17" t="n">
-        <v>-139657.2750165928</v>
+        <v>-14289.06734143041</v>
       </c>
       <c r="P17" t="n">
-        <v>0.9527735881763383</v>
+        <v>0.9530981600049149</v>
       </c>
       <c r="Q17" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R17" t="n">
-        <v>275220.3475144443</v>
+        <v>32078.95737517925</v>
       </c>
       <c r="S17" t="n">
-        <v>-76687.09179843753</v>
+        <v>-8626.403450231526</v>
       </c>
       <c r="T17" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U17" t="n">
-        <v>248626.7808909985</v>
+        <v>23626.76318557685</v>
       </c>
       <c r="V17" t="n">
-        <v>-77776.91764100146</v>
+        <v>-9013.606667623149</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B18" t="n">
-        <v>0.9510343339289785</v>
+        <v>0.9545093407777331</v>
       </c>
       <c r="C18" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D18" t="n">
-        <v>193820.0528968952</v>
+        <v>16501.23922446569</v>
       </c>
       <c r="E18" t="n">
-        <v>-18180.32721083442</v>
+        <v>-9035.270251842914</v>
       </c>
       <c r="F18" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G18" t="n">
-        <v>173454.9165805015</v>
+        <v>9704.534628774378</v>
       </c>
       <c r="H18" t="n">
-        <v>-18490.35429949855</v>
+        <v>-9489.992459225625</v>
       </c>
       <c r="I18" t="n">
-        <v>0.95396831505491</v>
+        <v>0.9543746754332608</v>
       </c>
       <c r="J18" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K18" t="n">
-        <v>162103.707301646</v>
+        <v>20573.08287393989</v>
       </c>
       <c r="L18" t="n">
-        <v>-138395.0098600878</v>
+        <v>-13845.72823880051</v>
       </c>
       <c r="M18" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N18" t="n">
-        <v>140636.1767574072</v>
+        <v>13740.27783596959</v>
       </c>
       <c r="O18" t="n">
-        <v>-139657.2750165928</v>
+        <v>-14289.06734143041</v>
       </c>
       <c r="P18" t="n">
-        <v>0.9527735881763383</v>
+        <v>0.9530981600049149</v>
       </c>
       <c r="Q18" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R18" t="n">
-        <v>275220.3475144443</v>
+        <v>32078.95737517925</v>
       </c>
       <c r="S18" t="n">
-        <v>-76687.09179843753</v>
+        <v>-8626.403450231526</v>
       </c>
       <c r="T18" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U18" t="n">
-        <v>248626.7808909985</v>
+        <v>23626.76318557685</v>
       </c>
       <c r="V18" t="n">
-        <v>-77776.91764100146</v>
+        <v>-9013.606667623149</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B19" t="n">
-        <v>0.9510343339289785</v>
+        <v>0.9545093407777331</v>
       </c>
       <c r="C19" t="n">
-        <v>212000.3801077296</v>
+        <v>25536.50947630861</v>
       </c>
       <c r="D19" t="n">
-        <v>193820.0528968952</v>
+        <v>16501.23922446569</v>
       </c>
       <c r="E19" t="n">
-        <v>-18180.32721083442</v>
+        <v>-9035.270251842914</v>
       </c>
       <c r="F19" t="n">
-        <v>191945.27088</v>
+        <v>19194.527088</v>
       </c>
       <c r="G19" t="n">
-        <v>173454.9165805015</v>
+        <v>9704.534628774378</v>
       </c>
       <c r="H19" t="n">
-        <v>-18490.35429949855</v>
+        <v>-9489.992459225625</v>
       </c>
       <c r="I19" t="n">
-        <v>0.95396831505491</v>
+        <v>0.9543746754332608</v>
       </c>
       <c r="J19" t="n">
-        <v>300498.7171617338</v>
+        <v>34418.8111127404</v>
       </c>
       <c r="K19" t="n">
-        <v>162103.707301646</v>
+        <v>20573.08287393989</v>
       </c>
       <c r="L19" t="n">
-        <v>-138395.0098600878</v>
+        <v>-13845.72823880051</v>
       </c>
       <c r="M19" t="n">
-        <v>280293.451774</v>
+        <v>28029.3451774</v>
       </c>
       <c r="N19" t="n">
-        <v>140636.1767574072</v>
+        <v>13740.27783596959</v>
       </c>
       <c r="O19" t="n">
-        <v>-139657.2750165928</v>
+        <v>-14289.06734143041</v>
       </c>
       <c r="P19" t="n">
-        <v>0.9527735881763383</v>
+        <v>0.9530981600049149</v>
       </c>
       <c r="Q19" t="n">
-        <v>351907.4393128818</v>
+        <v>40705.36082541077</v>
       </c>
       <c r="R19" t="n">
-        <v>275220.3475144443</v>
+        <v>32078.95737517925</v>
       </c>
       <c r="S19" t="n">
-        <v>-76687.09179843753</v>
+        <v>-8626.403450231526</v>
       </c>
       <c r="T19" t="n">
-        <v>326403.698532</v>
+        <v>32640.3698532</v>
       </c>
       <c r="U19" t="n">
-        <v>248626.7808909985</v>
+        <v>23626.76318557685</v>
       </c>
       <c r="V19" t="n">
-        <v>-77776.91764100146</v>
+        <v>-9013.606667623149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>